<commit_message>
Added: Option to saveData
</commit_message>
<xml_diff>
--- a/Excell and Manipulation Function/Testes.xlsx
+++ b/Excell and Manipulation Function/Testes.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Users\benvi\OneDrive\Documents\NetBeansProjects\9CARDSIEGE_PA\Neural-Network---Matlab\Neural-Network---Matlab\Excell and Manipulation Function\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Neural-Network---Matlab\Excell and Manipulation Function\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF7061FE-CB6A-445E-B93B-FDFA5ECBE2BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ex1_a)" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="71">
   <si>
     <t>Funções de ativação</t>
   </si>
@@ -250,7 +249,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -737,10 +736,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -1531,11 +1530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2689,9 +2688,7 @@
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
@@ -2710,7 +2707,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2722,7 +2719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>